<commit_message>
Record updated perf in excel spreadsheet
</commit_message>
<xml_diff>
--- a/graph.xlsx
+++ b/graph.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21310"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\MessagePack-CSharp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C89E4D-52EA-4D61-B931-0C492B106DB4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364D8BDB-8306-4FEC-ACE3-2B899A73A5C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48480" yWindow="-3600" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2820" yWindow="3330" windowWidth="21990" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README graph" sheetId="2" r:id="rId1"/>
@@ -47,39 +47,39 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
   <si>
     <t>Small Object(int, string, stringm enum)</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>MessagePack C#</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>MsgPack-Cli</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>protobuf-net</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>ZeroFormatter</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>Serialize</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>Deserialize</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>FileSize</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>Large Array(Small Object[1000])</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>protobuf-net</t>
@@ -112,7 +112,7 @@
     <t>Json.NET(+GZip)</t>
   </si>
   <si>
-    <t>c405c58cbf (origin/master)</t>
+    <t>v2.0 (df8cc0f25)</t>
   </si>
 </sst>
 </file>
@@ -120,8 +120,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="0\ &quot;bytes&quot;"/>
-    <numFmt numFmtId="165" formatCode="#,#00\ &quot;ms&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,#00\ &quot;ms&quot;"/>
+    <numFmt numFmtId="165" formatCode="#,#00\ &quot;bytes&quot;"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -140,17 +140,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="6"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -174,18 +175,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -332,25 +334,25 @@
                 <c:formatCode>#,#00\ "ms"</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>137.69999999999999</c:v>
+                  <c:v>112.64</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>160.72999999999999</c:v>
+                  <c:v>133.41999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>335.23</c:v>
+                  <c:v>290.95999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>449.62</c:v>
+                  <c:v>435.66</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>141.72999999999999</c:v>
+                  <c:v>108.12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1543.3</c:v>
+                  <c:v>965.99</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1680.56</c:v>
+                  <c:v>1404.07</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -384,25 +386,25 @@
                 <c:formatCode>#,#00\ "ms"</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>177.33</c:v>
+                  <c:v>213.95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>182.04</c:v>
+                  <c:v>227.84</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1106.8699999999999</c:v>
+                  <c:v>909.12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>627.23</c:v>
+                  <c:v>584.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>139.91</c:v>
+                  <c:v>118.26</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1876.02</c:v>
+                  <c:v>1862.41</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2237.38</c:v>
+                  <c:v>2031.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -470,13 +472,13 @@
             <c:numRef>
               <c:f>'README graph'!$B$21:$B$27</c:f>
               <c:numCache>
-                <c:formatCode>0\ "bytes"</c:formatCode>
+                <c:formatCode>#,#00\ "bytes"</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1803</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>562</c:v>
+                  <c:v>563</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2347</c:v>
@@ -589,6 +591,31 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -660,7 +687,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
-        <c:numFmt formatCode="0\ &quot;bytes&quot;" sourceLinked="1"/>
+        <c:numFmt formatCode="#,#00\ &quot;bytes&quot;" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3917,16 +3944,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>100013</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>271463</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4347,18 +4374,18 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.46484375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.06640625" style="1"/>
+    <col min="1" max="1" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>19</v>
       </c>
     </row>
@@ -4368,188 +4395,188 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="4">
-        <v>137.69999999999999</v>
+      <c r="B3" s="3">
+        <v>112.64</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="4">
-        <v>160.72999999999999</v>
+      <c r="B4" s="3">
+        <v>133.41999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="4">
-        <v>335.23</v>
+      <c r="B5" s="3">
+        <v>290.95999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="4">
-        <v>449.62</v>
+      <c r="B6" s="3">
+        <v>435.66</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="4">
-        <v>141.72999999999999</v>
+      <c r="B7" s="3">
+        <v>108.12</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="4">
-        <v>1543.3</v>
+      <c r="B8" s="3">
+        <v>965.99</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="4">
-        <v>1680.56</v>
+      <c r="B9" s="3">
+        <v>1404.07</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="3"/>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="3"/>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="4">
-        <v>177.33</v>
+      <c r="B12" s="3">
+        <v>213.95</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="4">
-        <v>182.04</v>
+      <c r="B13" s="3">
+        <v>227.84</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="4">
-        <v>1106.8699999999999</v>
+      <c r="B14" s="3">
+        <v>909.12</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="4">
-        <v>627.23</v>
+      <c r="B15" s="3">
+        <v>584.5</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="4">
-        <v>139.91</v>
+      <c r="B16" s="3">
+        <v>118.26</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="4">
-        <v>1876.02</v>
+      <c r="B17" s="3">
+        <v>1862.41</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="4">
-        <v>2237.38</v>
+      <c r="B18" s="3">
+        <v>2031.4</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="3"/>
+      <c r="A19" s="2"/>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="4">
         <v>1803</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="2">
-        <v>562</v>
+      <c r="B22" s="4">
+        <v>563</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="4">
         <v>2347</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="4">
         <v>2248</v>
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="4">
         <v>5004</v>
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="4">
         <v>6096</v>
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="4">
         <v>458</v>
       </c>
     </row>
@@ -4569,9 +4596,9 @@
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="8" max="8" width="10.46484375" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="8" spans="8:12">
@@ -4715,7 +4742,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2"/>
+  <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Update Excel spreadsheet and README graphic
</commit_message>
<xml_diff>
--- a/graph.xlsx
+++ b/graph.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21310"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\MessagePack-CSharp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\MessagePack-CSharp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C89E4D-52EA-4D61-B931-0C492B106DB4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F14620-0BB8-47E4-B0F1-3ED9A04F30ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48480" yWindow="-3600" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6990" yWindow="1785" windowWidth="29100" windowHeight="17085" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README graph" sheetId="2" r:id="rId1"/>
@@ -28,15 +28,32 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={675115CE-AC10-4A12-9B1A-05563BDC58F9}</author>
+    <author>Andrew Arnott</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{675115CE-AC10-4A12-9B1A-05563BDC58F9}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{DE293BED-DF5D-4D85-B9D9-DDDD79E5E60C}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Regenerate/refresh this data using the sandbox\PerfNetFramework program.</t>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Andrew Arnott:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Regenerate/refresh this data using the sandbox\PerfNetFramework program:
+dotnet run -c release -p sandbox\PerfNetFramework -f netcoreapp3.1</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -44,42 +61,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
   <si>
     <t>Small Object(int, string, stringm enum)</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="4"/>
   </si>
   <si>
     <t>MessagePack C#</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="4"/>
   </si>
   <si>
     <t>MsgPack-Cli</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="4"/>
   </si>
   <si>
     <t>protobuf-net</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="4"/>
   </si>
   <si>
     <t>ZeroFormatter</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="4"/>
   </si>
   <si>
     <t>Serialize</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="4"/>
   </si>
   <si>
     <t>Deserialize</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="4"/>
   </si>
   <si>
     <t>FileSize</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="4"/>
   </si>
   <si>
     <t>Large Array(Small Object[1000])</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="4"/>
   </si>
   <si>
     <t>protobuf-net</t>
@@ -112,7 +129,10 @@
     <t>Json.NET(+GZip)</t>
   </si>
   <si>
-    <t>c405c58cbf (origin/master)</t>
+    <t>OdinSerializer</t>
+  </si>
+  <si>
+    <t>98cb21e729002d (origin/master)</t>
   </si>
 </sst>
 </file>
@@ -123,13 +143,27 @@
     <numFmt numFmtId="164" formatCode="0\ &quot;bytes&quot;"/>
     <numFmt numFmtId="165" formatCode="#,#00\ &quot;ms&quot;"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -150,7 +184,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -174,18 +215,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -239,8 +284,21 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Person[100], 10K iterations</a:t>
+              <a:t>SmallObject[1000]</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> array</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>, NET</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Core 3.1</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -298,9 +356,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'README graph'!$A$3:$A$9</c:f>
+              <c:f>'README graph'!$A$3:$A$10</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>MessagePack for C#</c:v>
                 </c:pt>
@@ -317,9 +375,12 @@
                   <c:v>ZeroFormatter</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>OdinSerializer</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>Json.NET</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Json.NET(+GZip)</c:v>
                 </c:pt>
               </c:strCache>
@@ -327,30 +388,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'README graph'!$B$3:$B$9</c:f>
+              <c:f>'README graph'!$B$3:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>#,#00\ "ms"</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>137.69999999999999</c:v>
+                  <c:v>96.59</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>160.72999999999999</c:v>
+                  <c:v>119.73</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>335.23</c:v>
+                  <c:v>219.89</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>449.62</c:v>
+                  <c:v>186.98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>141.72999999999999</c:v>
+                  <c:v>97.12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1543.3</c:v>
+                  <c:v>796.61</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1680.56</c:v>
+                  <c:v>815.69</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1014.89</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -379,30 +443,33 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'README graph'!$B$12:$B$18</c:f>
+              <c:f>'README graph'!$B$13:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>#,#00\ "ms"</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>177.33</c:v>
+                  <c:v>170.98</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>182.04</c:v>
+                  <c:v>178.57</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1106.8699999999999</c:v>
+                  <c:v>483.38</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>627.23</c:v>
+                  <c:v>186.78</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>139.91</c:v>
+                  <c:v>96.48</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1876.02</c:v>
+                  <c:v>1772.4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2237.38</c:v>
+                  <c:v>1825.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1894.96</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -433,7 +500,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'README graph'!$A$20</c:f>
+              <c:f>'README graph'!$A$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -468,15 +535,15 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'README graph'!$B$21:$B$27</c:f>
+              <c:f>'README graph'!$B$23:$B$30</c:f>
               <c:numCache>
                 <c:formatCode>0\ "bytes"</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1803</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>562</c:v>
+                  <c:v>560</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2347</c:v>
@@ -488,10 +555,13 @@
                   <c:v>5004</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>26699</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>6096</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>458</c:v>
+                <c:pt idx="7">
+                  <c:v>464</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -589,6 +659,31 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Total time, 10K iterations</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3917,16 +4012,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>304799</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>100013</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4031,12 +4126,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Andrew Arnott" id="{741C964C-831C-49B3-8C72-00961BB146EB}" userId="S::andarno@microsoft.com::fef1612b-3282-4fb1-9982-6bb0b7d12ab8" providerId="AD"/>
-</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4334,32 +4423,24 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="B1" dT="2019-01-27T03:35:00.29" personId="{741C964C-831C-49B3-8C72-00961BB146EB}" id="{675115CE-AC10-4A12-9B1A-05563BDC58F9}">
-    <text>Regenerate/refresh this data using the sandbox\PerfNetFramework program.</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C478671A-2BFF-4005-AC60-F5FFFBF24A55}">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.46484375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.06640625" style="1"/>
+    <col min="1" max="1" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="B1" s="1" t="s">
-        <v>19</v>
+      <c r="B1" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -4372,7 +4453,7 @@
         <v>15</v>
       </c>
       <c r="B3" s="4">
-        <v>137.69999999999999</v>
+        <v>96.59</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -4380,7 +4461,7 @@
         <v>16</v>
       </c>
       <c r="B4" s="4">
-        <v>160.72999999999999</v>
+        <v>119.73</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -4388,7 +4469,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="4">
-        <v>335.23</v>
+        <v>219.89</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4396,7 +4477,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="4">
-        <v>449.62</v>
+        <v>186.98</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -4404,153 +4485,177 @@
         <v>10</v>
       </c>
       <c r="B7" s="4">
-        <v>141.72999999999999</v>
+        <v>97.12</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="3" t="s">
-        <v>17</v>
+      <c r="A8" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="B8" s="4">
-        <v>1543.3</v>
+        <v>796.61</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="4">
-        <v>1680.56</v>
+        <v>815.69</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
+      <c r="A10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="4">
+        <v>1014.89</v>
+      </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="A11" s="3"/>
       <c r="B11" s="4"/>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="4">
-        <v>177.33</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="B12" s="4"/>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="4">
-        <v>182.04</v>
+        <v>170.98</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B14" s="4">
-        <v>1106.8699999999999</v>
+        <v>178.57</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B15" s="4">
-        <v>627.23</v>
+        <v>483.38</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16" s="4">
-        <v>139.91</v>
+        <v>186.78</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="3" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B17" s="4">
-        <v>1876.02</v>
+        <v>96.48</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="3" t="s">
-        <v>18</v>
+      <c r="A18" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="B18" s="4">
-        <v>2237.38</v>
+        <v>1772.4</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="3"/>
+      <c r="A19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="4">
+        <v>1825.7</v>
+      </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="3" t="s">
-        <v>12</v>
+        <v>18</v>
+      </c>
+      <c r="B20" s="4">
+        <v>1894.96</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" s="2">
-        <v>1803</v>
-      </c>
+      <c r="A21" s="3"/>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" s="2">
-        <v>562</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B23" s="2">
-        <v>2347</v>
+        <v>1803</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="3" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B24" s="2">
-        <v>2248</v>
+        <v>560</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B25" s="2">
-        <v>5004</v>
+        <v>2347</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B26" s="2">
-        <v>6096</v>
+        <v>2248</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="2">
+        <v>5004</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="2">
+        <v>26699</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="2">
+        <v>6096</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B27" s="2">
-        <v>458</v>
+      <c r="B30" s="2">
+        <v>464</v>
       </c>
     </row>
   </sheetData>
@@ -4569,9 +4674,9 @@
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="8" max="8" width="10.46484375" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="8" spans="8:12">
@@ -4715,9 +4820,15 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2"/>
+  <phoneticPr fontId="4"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Privileged" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>